<commit_message>
new commit on 16th sep
</commit_message>
<xml_diff>
--- a/git commands.xlsx
+++ b/git commands.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shashankjain/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shashankjain/Desktop/Imp_notes/Summary_notes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC7384A7-4CA1-4440-A598-B3A14B3060A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C785A62F-D363-D940-AAFF-4110D4FCA840}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{9654F469-6A19-CB40-8C72-7E8BC39600D7}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{9654F469-6A19-CB40-8C72-7E8BC39600D7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="81">
   <si>
     <t>List of file in git staging area</t>
   </si>
@@ -315,6 +315,18 @@
   </si>
   <si>
     <t>will return last commit of local and remote branches.  With this command you can check if local &amp; remote are in sync or not.</t>
+  </si>
+  <si>
+    <t>git commit --amend --author="shashanknew47&lt;shashank.edu@gmail.com&gt;"</t>
+  </si>
+  <si>
+    <t>git config user.name "shashanknew47"</t>
+  </si>
+  <si>
+    <t>git config user.email "shashank.edu@gmail.com"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">git config --list </t>
   </si>
 </sst>
 </file>
@@ -358,13 +370,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -381,6 +399,107 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>112059</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>7472</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>9435352</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>1277471</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BCF349B3-A983-2F45-120E-52706AAF64C8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2906059" y="14044707"/>
+          <a:ext cx="9323293" cy="1269999"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>If you want to change the name of commiter and email in the commit. Then </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>=&gt; first</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" baseline="0"/>
+            <a:t> login in with username and username what you want to change with :</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" baseline="0"/>
+            <a:t>      - git config user.name "shashank47.edu@gmail.com"</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" baseline="0"/>
+            <a:t>         git config user.email "shashank.edu@gmail.com"</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-GB" sz="1100" baseline="0"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -680,341 +799,363 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24A8B4CD-778B-384E-BBC1-8AC8C3D0AE3B}">
-  <dimension ref="A2:B63"/>
+  <dimension ref="A1:B69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="A66" sqref="A66"/>
+    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="39.33203125" customWidth="1"/>
+    <col min="1" max="1" width="42.33203125" customWidth="1"/>
     <col min="2" max="2" width="131.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>0</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>29</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B10" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B14" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>21</v>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B19" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>24</v>
-      </c>
-      <c r="B20" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
         <v>27</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B25" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="34" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+    <row r="28" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
         <v>31</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B28" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
         <v>30</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B29" t="s">
         <v>33</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>39</v>
-      </c>
-      <c r="B27" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>41</v>
-      </c>
-      <c r="B28" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B30" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B31" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" ht="34" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>36</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>35</v>
+      </c>
       <c r="B33" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
+        <v>43</v>
+      </c>
+      <c r="B34" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>36</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B36" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
         <v>45</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B37" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
         <v>57</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B38" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
         <v>47</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B39" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A39" s="2" t="s">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B42" t="s">
         <v>50</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A40" s="2"/>
-      <c r="B40" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A41" s="2"/>
-      <c r="B41" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A42" s="2"/>
-      <c r="B42" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" s="2"/>
       <c r="B43" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" s="2"/>
+      <c r="B44" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" s="2"/>
+      <c r="B45" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46" s="2"/>
+      <c r="B46" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B44" t="s">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B47" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B45" t="s">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B48" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
         <v>59</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B51" t="s">
         <v>60</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
-        <v>61</v>
-      </c>
-      <c r="B50" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B53" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" ht="34" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
-        <v>65</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
+        <v>63</v>
+      </c>
+      <c r="B56" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>65</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
         <v>67</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B59" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="59" spans="1:2" ht="34" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
+    <row r="62" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
         <v>69</v>
       </c>
-      <c r="B59" s="1" t="s">
+      <c r="B62" s="1" t="s">
         <v>70</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
-        <v>71</v>
-      </c>
-      <c r="B60" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
-        <v>73</v>
-      </c>
-      <c r="B62" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
+        <v>71</v>
+      </c>
+      <c r="B63" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>73</v>
+      </c>
+      <c r="B65" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
         <v>75</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B66" t="s">
         <v>76</v>
       </c>
+    </row>
+    <row r="69" spans="1:2" ht="105" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A69" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B69" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A39:A43"/>
+    <mergeCell ref="A42:A46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>